<commit_message>
final story edits before recording
</commit_message>
<xml_diff>
--- a/story_xlsx_files_postpilotiiedits/11.xlsx
+++ b/story_xlsx_files_postpilotiiedits/11.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>storyText</t>
   </si>
@@ -40,59 +40,37 @@
   <si>
     <r>
       <rPr>
-        <b val="1"/>
-        <sz val="10"/>
+        <sz val="16"/>
         <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
+        <rFont val="Arial"/>
       </rPr>
-      <t>T</t>
+      <t xml:space="preserve">A bell chimed as the door swung open, and Sadie entered to find Thomas, who was </t>
     </r>
     <r>
       <rPr>
-        <b val="1"/>
-        <sz val="10"/>
+        <sz val="16"/>
         <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
+        <rFont val="Arial"/>
       </rPr>
-      <t>h</t>
+      <t>dreading the approaching breakup conversation he was about to start,</t>
     </r>
     <r>
       <rPr>
-        <b val="1"/>
-        <sz val="10"/>
+        <sz val="16"/>
         <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
+        <rFont val="Arial"/>
       </rPr>
-      <t xml:space="preserve">omas, dreading the approaching breakup conversation he was about to start, got to </t>
+      <t xml:space="preserve"> ruminating at the bar.</t>
     </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <i val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>Annika’s Finer Diner</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve"> late but Sadie, his girlfriend, was not there yet.</t>
-    </r>
   </si>
   <si>
     <t>Thomas had been thinking about breaking up with her for 2 months now.</t>
   </si>
   <si>
-    <t xml:space="preserve">The restaurant he had chosen to meet at was reminiscent of a diner from the 70’s with black and white checkerboard tiling on the floor, a long bar in the front, and booths and stools with red, leather upholstery. </t>
-  </si>
-  <si>
-    <t>A bell chimed as the door swung open, and Sadie entered to find Thomas ruminating at the bar.</t>
+    <t>The restaurant, Annika’s Finer Diner, he had chosen to meet at was reminiscent of a diner from the 70’s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There were black and white checkerboard tiling on the floor, a long bar in the front, and booths and stools with red, leather upholstery. </t>
   </si>
   <si>
     <t>He stood up and gave her a side hug, asking quickly, “How was your day?”</t>
@@ -129,9 +107,6 @@
   </si>
   <si>
     <t>“Tell me about your day!” she sang.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">He looked at her silently and pulled his hand slowly from hers as a puzzled look grew on Sadie’s face. </t>
   </si>
   <si>
     <t xml:space="preserve">Thomas looked away and took a deep breath. </t>
@@ -358,7 +333,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -371,13 +346,6 @@
     </font>
     <font>
       <b val="1"/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -537,8 +505,8 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -561,7 +529,7 @@
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1646,7 +1614,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
@@ -1684,7 +1652,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="128.25" customHeight="1">
+    <row r="2" ht="350" customHeight="1">
       <c r="A2" t="s" s="3">
         <v>8</v>
       </c>
@@ -1696,9 +1664,7 @@
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="5">
-        <v>11</v>
-      </c>
+      <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
     </row>
@@ -1720,7 +1686,7 @@
       </c>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" ht="176.05" customHeight="1">
+    <row r="4" ht="92.05" customHeight="1">
       <c r="A4" t="s" s="7">
         <v>10</v>
       </c>
@@ -1738,8 +1704,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="187.8" customHeight="1">
-      <c r="A5" t="s" s="11">
+    <row r="5" ht="116.05" customHeight="1">
+      <c r="A5" t="s" s="7">
         <v>11</v>
       </c>
       <c r="B5" s="8">
@@ -1868,7 +1834,7 @@
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
     </row>
-    <row r="13" ht="187.8" customHeight="1">
+    <row r="13" ht="97.8" customHeight="1">
       <c r="A13" t="s" s="11">
         <v>19</v>
       </c>
@@ -1884,7 +1850,7 @@
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" ht="97.8" customHeight="1">
+    <row r="14" ht="79.8" customHeight="1">
       <c r="A14" t="s" s="11">
         <v>20</v>
       </c>
@@ -1900,7 +1866,7 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
     </row>
-    <row r="15" ht="79.8" customHeight="1">
+    <row r="15" ht="61.8" customHeight="1">
       <c r="A15" t="s" s="11">
         <v>21</v>
       </c>
@@ -1911,12 +1877,14 @@
         <v>1</v>
       </c>
       <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="9">
+        <v>22</v>
+      </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" ht="61.8" customHeight="1">
+    <row r="16" ht="331.8" customHeight="1">
       <c r="A16" t="s" s="11">
         <v>22</v>
       </c>
@@ -1924,17 +1892,15 @@
         <v>2</v>
       </c>
       <c r="C16" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="10"/>
-      <c r="E16" s="9">
-        <v>22</v>
-      </c>
+      <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" ht="331.8" customHeight="1">
+    <row r="17" ht="61.8" customHeight="1">
       <c r="A17" t="s" s="11">
         <v>23</v>
       </c>
@@ -1950,7 +1916,7 @@
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
     </row>
-    <row r="18" ht="61.8" customHeight="1">
+    <row r="18" ht="223.8" customHeight="1">
       <c r="A18" t="s" s="11">
         <v>24</v>
       </c>
@@ -1966,7 +1932,7 @@
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
     </row>
-    <row r="19" ht="223.8" customHeight="1">
+    <row r="19" ht="241.8" customHeight="1">
       <c r="A19" t="s" s="11">
         <v>25</v>
       </c>
@@ -1976,31 +1942,31 @@
       <c r="C19" s="9">
         <v>2</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="9">
+        <v>17</v>
+      </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
     </row>
-    <row r="20" ht="241.8" customHeight="1">
+    <row r="20" ht="151.8" customHeight="1">
       <c r="A20" t="s" s="11">
         <v>26</v>
       </c>
       <c r="B20" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20" s="9">
         <v>2</v>
       </c>
-      <c r="D20" s="9">
-        <v>17</v>
-      </c>
+      <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
     </row>
-    <row r="21" ht="151.8" customHeight="1">
+    <row r="21" ht="187.8" customHeight="1">
       <c r="A21" t="s" s="11">
         <v>27</v>
       </c>
@@ -2016,7 +1982,7 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" ht="187.8" customHeight="1">
+    <row r="22" ht="295.8" customHeight="1">
       <c r="A22" t="s" s="11">
         <v>28</v>
       </c>
@@ -2032,7 +1998,7 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
     </row>
-    <row r="23" ht="295.8" customHeight="1">
+    <row r="23" ht="97.8" customHeight="1">
       <c r="A23" t="s" s="11">
         <v>29</v>
       </c>
@@ -2048,7 +2014,7 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
     </row>
-    <row r="24" ht="97.8" customHeight="1">
+    <row r="24" ht="133.8" customHeight="1">
       <c r="A24" t="s" s="11">
         <v>30</v>
       </c>
@@ -2080,7 +2046,7 @@
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
     </row>
-    <row r="26" ht="133.8" customHeight="1">
+    <row r="26" ht="79.8" customHeight="1">
       <c r="A26" t="s" s="11">
         <v>32</v>
       </c>
@@ -2088,7 +2054,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -2096,7 +2062,7 @@
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
     </row>
-    <row r="27" ht="79.8" customHeight="1">
+    <row r="27" ht="187.8" customHeight="1">
       <c r="A27" t="s" s="11">
         <v>33</v>
       </c>
@@ -2112,7 +2078,7 @@
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
     </row>
-    <row r="28" ht="187.8" customHeight="1">
+    <row r="28" ht="97.8" customHeight="1">
       <c r="A28" t="s" s="11">
         <v>34</v>
       </c>
@@ -2144,7 +2110,7 @@
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
     </row>
-    <row r="30" ht="97.8" customHeight="1">
+    <row r="30" ht="151.8" customHeight="1">
       <c r="A30" t="s" s="11">
         <v>36</v>
       </c>
@@ -2160,7 +2126,7 @@
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
     </row>
-    <row r="31" ht="151.8" customHeight="1">
+    <row r="31" ht="115.8" customHeight="1">
       <c r="A31" t="s" s="11">
         <v>37</v>
       </c>
@@ -2176,7 +2142,7 @@
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
     </row>
-    <row r="32" ht="115.8" customHeight="1">
+    <row r="32" ht="151.8" customHeight="1">
       <c r="A32" t="s" s="11">
         <v>38</v>
       </c>
@@ -2186,7 +2152,9 @@
       <c r="C32" s="9">
         <v>3</v>
       </c>
-      <c r="D32" s="10"/>
+      <c r="D32" s="9">
+        <v>20</v>
+      </c>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
@@ -2197,20 +2165,18 @@
         <v>39</v>
       </c>
       <c r="B33" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C33" s="9">
         <v>3</v>
       </c>
-      <c r="D33" s="9">
-        <v>20</v>
-      </c>
+      <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
     </row>
-    <row r="34" ht="151.8" customHeight="1">
+    <row r="34" ht="97.8" customHeight="1">
       <c r="A34" t="s" s="11">
         <v>40</v>
       </c>
@@ -2258,7 +2224,7 @@
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
     </row>
-    <row r="37" ht="97.8" customHeight="1">
+    <row r="37" ht="295.8" customHeight="1">
       <c r="A37" t="s" s="11">
         <v>43</v>
       </c>
@@ -2266,7 +2232,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
@@ -2274,7 +2240,7 @@
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
     </row>
-    <row r="38" ht="295.8" customHeight="1">
+    <row r="38" ht="115.8" customHeight="1">
       <c r="A38" t="s" s="11">
         <v>44</v>
       </c>
@@ -2290,7 +2256,7 @@
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
     </row>
-    <row r="39" ht="115.8" customHeight="1">
+    <row r="39" ht="169.8" customHeight="1">
       <c r="A39" t="s" s="11">
         <v>45</v>
       </c>
@@ -2306,7 +2272,7 @@
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
     </row>
-    <row r="40" ht="169.8" customHeight="1">
+    <row r="40" ht="151.8" customHeight="1">
       <c r="A40" t="s" s="11">
         <v>46</v>
       </c>
@@ -2322,7 +2288,7 @@
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" ht="151.8" customHeight="1">
+    <row r="41" ht="169.8" customHeight="1">
       <c r="A41" t="s" s="11">
         <v>47</v>
       </c>
@@ -2338,7 +2304,7 @@
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
     </row>
-    <row r="42" ht="169.8" customHeight="1">
+    <row r="42" ht="205.8" customHeight="1">
       <c r="A42" t="s" s="11">
         <v>48</v>
       </c>
@@ -2348,31 +2314,15 @@
       <c r="C42" s="9">
         <v>4</v>
       </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
+      <c r="D42" s="9">
+        <v>13</v>
+      </c>
+      <c r="E42" s="9">
+        <v>5</v>
+      </c>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
-    </row>
-    <row r="43" ht="205.8" customHeight="1">
-      <c r="A43" t="s" s="11">
-        <v>49</v>
-      </c>
-      <c r="B43" s="8">
-        <v>4</v>
-      </c>
-      <c r="C43" s="9">
-        <v>4</v>
-      </c>
-      <c r="D43" s="9">
-        <v>13</v>
-      </c>
-      <c r="E43" s="9">
-        <v>5</v>
-      </c>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>